<commit_message>
set src language to english in expand_keywords.py
</commit_message>
<xml_diff>
--- a/keywords/keywords.xlsx
+++ b/keywords/keywords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c0ac04fbadbefb8/SDG/Policy-Mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c0ac04fbadbefb8/SDG/Policy-Mapping/keywords/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{7DC56746-C8C4-47E0-81EA-8E939D54C9FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A1DFC776-96C4-4C69-BEFA-C0D3754BB3FC}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{7DC56746-C8C4-47E0-81EA-8E939D54C9FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{988D9236-E7EB-4841-A411-85306356100D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -835,9 +835,6 @@
     <t>cocoa prices;prices of cocoa;</t>
   </si>
   <si>
-    <t>international poverty line;extreme poverty;abject poverty;absolute poverty;destitution;penury;severe deprivation;help people suffering from food and material deprivation;extremely poor;incidence of poverty;Households in poverty;</t>
-  </si>
-  <si>
     <t>poverty reduction programmes;means for developing countries;reduce poverty in developing countries;reduce poverty LDCs;development assistance grants from all donors that focus on poverty reduction;development assistance for poverty reduction;</t>
   </si>
   <si>
@@ -1444,6 +1441,9 @@
   </si>
   <si>
     <t>healthy ocean;productive ocean;marine ecosystem;coastal ecosystem;marine protected area;marine biodiversity;sustainable management of oceanic and coastal fisheries;protect lives and livelihoods in coastal areas;integrated costal management;water management in the sea basin;sustainable marine environments;sustainable maritime transport;coastal biodiversity;loss of coastal habitats;marine key biodiversity areas;conserve oceans;oceans must be conserved;sustainable development of water ecosystems;protection of water and marine resources;conserve seas;conserve marine resources;protect oceans;protect seas;protect marine resources;</t>
+  </si>
+  <si>
+    <t>international poverty line; extreme poverty; abject poverty; absolute poverty;destitution;penury;severe deprivation;help people suffering from food and material deprivation;extremely poor;incidence of poverty;Households in poverty;</t>
   </si>
 </sst>
 </file>
@@ -2037,10 +2037,10 @@
   <dimension ref="A1:J170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B119" sqref="B119"/>
+      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>265</v>
+        <v>467</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>208</v>
@@ -2105,7 +2105,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2113,7 +2113,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2121,7 +2121,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>215</v>
@@ -2148,7 +2148,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>218</v>
@@ -2159,7 +2159,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J9" s="37" t="s">
         <v>261</v>
@@ -2170,7 +2170,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2178,7 +2178,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2186,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2194,7 +2194,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J14" s="37" t="s">
         <v>262</v>
@@ -2213,7 +2213,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H15" s="35" t="s">
         <v>263</v>
@@ -2224,7 +2224,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H16" s="35" t="s">
         <v>264</v>
@@ -2235,7 +2235,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2243,7 +2243,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2251,10 +2251,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="J19" s="37" t="s">
         <v>434</v>
-      </c>
-      <c r="J19" s="37" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2270,7 +2270,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2278,7 +2278,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2286,7 +2286,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2294,7 +2294,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2310,7 +2310,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>223</v>
@@ -2369,7 +2369,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>251</v>
@@ -2388,7 +2388,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>220</v>
@@ -2399,7 +2399,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>221</v>
@@ -2410,7 +2410,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>222</v>
@@ -2421,7 +2421,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2429,7 +2429,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2445,7 +2445,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2453,7 +2453,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2461,7 +2461,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2469,7 +2469,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2501,7 +2501,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2509,7 +2509,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2525,7 +2525,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2533,7 +2533,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2573,7 +2573,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2589,7 +2589,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2597,7 +2597,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2613,7 +2613,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2621,7 +2621,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -2645,7 +2645,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -2653,7 +2653,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C67"/>
       <c r="D67"/>
@@ -2669,7 +2669,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -2677,7 +2677,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -2685,7 +2685,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -2693,7 +2693,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -2701,7 +2701,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -2709,7 +2709,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -2725,7 +2725,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -2733,7 +2733,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -2741,10 +2741,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J77" s="34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -2752,7 +2752,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2760,10 +2760,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="J79" s="34" t="s">
         <v>307</v>
-      </c>
-      <c r="J79" s="34" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2771,7 +2771,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2779,7 +2779,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>228</v>
@@ -2798,7 +2798,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2822,7 +2822,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2830,7 +2830,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>229</v>
@@ -2841,7 +2841,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>230</v>
@@ -2852,7 +2852,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>231</v>
@@ -2863,7 +2863,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2879,7 +2879,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2887,7 +2887,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2895,7 +2895,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2903,7 +2903,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2911,7 +2911,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -2919,7 +2919,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
@@ -2927,7 +2927,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -2935,7 +2935,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
@@ -2943,7 +2943,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -2959,7 +2959,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
@@ -2967,7 +2967,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C103" s="15" t="s">
         <v>235</v>
@@ -2978,7 +2978,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="106" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3010,7 +3010,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C109" s="15" t="s">
         <v>236</v>
@@ -3048,7 +3048,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -3080,7 +3080,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -3088,7 +3088,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -3104,7 +3104,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -3128,7 +3128,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -3136,7 +3136,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -3144,7 +3144,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -3152,7 +3152,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -3160,7 +3160,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -3168,7 +3168,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -3176,7 +3176,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -3184,7 +3184,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3192,7 +3192,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C129" s="15" t="s">
         <v>243</v>
@@ -3203,7 +3203,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C130" s="15" t="s">
         <v>244</v>
@@ -3214,7 +3214,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C131" s="15" t="s">
         <v>245</v>
@@ -3225,7 +3225,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C132" s="15" t="s">
         <v>246</v>
@@ -3236,7 +3236,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C133" s="15" t="s">
         <v>247</v>
@@ -3247,7 +3247,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D134" s="31" t="s">
         <v>242</v>
@@ -3258,7 +3258,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -3266,7 +3266,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C136" s="15" t="s">
         <v>240</v>
@@ -3277,7 +3277,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C137" s="15" t="s">
         <v>248</v>
@@ -3288,13 +3288,13 @@
         <v>136</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C138" s="15" t="s">
         <v>249</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C139" s="15" t="s">
         <v>250</v>
@@ -3313,7 +3313,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,7 +3321,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3329,7 +3329,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3353,7 +3353,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
@@ -3361,7 +3361,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
@@ -3369,7 +3369,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
@@ -3377,7 +3377,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
@@ -3385,7 +3385,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
@@ -3393,7 +3393,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I153" s="38"/>
     </row>
@@ -3426,7 +3426,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C154" s="15"/>
       <c r="D154" s="12"/>
@@ -3442,7 +3442,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
@@ -3450,7 +3450,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
@@ -3458,7 +3458,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
@@ -3466,7 +3466,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
@@ -3482,7 +3482,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3490,7 +3490,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -3498,7 +3498,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3514,7 +3514,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3522,7 +3522,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3530,7 +3530,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3538,7 +3538,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3554,7 +3554,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3562,7 +3562,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3626,10 +3626,10 @@
     </row>
     <row r="2" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>214</v>
@@ -3643,10 +3643,10 @@
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L3" s="30" t="s">
         <v>226</v>
@@ -3655,10 +3655,10 @@
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>238</v>
@@ -3666,10 +3666,10 @@
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>219</v>
@@ -3677,10 +3677,10 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>233</v>
@@ -3688,42 +3688,42 @@
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>232</v>
@@ -3731,18 +3731,18 @@
     </row>
     <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>237</v>
@@ -3750,26 +3750,26 @@
     </row>
     <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>241</v>
@@ -3777,10 +3777,10 @@
     </row>
     <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>239</v>
@@ -3788,10 +3788,10 @@
     </row>
     <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3902,7 +3902,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3943,7 +3943,7 @@
         <v>153</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3951,7 +3951,7 @@
         <v>154</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3959,7 +3959,7 @@
         <v>156</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented horizontal, vertical, circular targetplot. Added collapse_keywords script in misc/.
</commit_message>
<xml_diff>
--- a/keywords/keywords.xlsx
+++ b/keywords/keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_JRC\Mapping_2\Keywords\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EB7C7-91C0-4A33-9689-A106948B7AF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F01615-3BE2-4C2A-B3E7-D1DA3AFF051A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target_keys" sheetId="1" r:id="rId1"/>
@@ -2172,20 +2172,20 @@
       <selection pane="bottomRight" activeCell="B61" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="12" customWidth="1"/>
     <col min="5" max="5" width="18" style="17" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="12" customWidth="1"/>
     <col min="8" max="8" width="18" style="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>169</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>5</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>6</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>15</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>16</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>17</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>18</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>20</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>21</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>22</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>23</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>24</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>25</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>27</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>28</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>29</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>30</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>31</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>32</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>33</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>34</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>35</v>
       </c>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>36</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>37</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>38</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>39</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>40</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>41</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>43</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>44</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>45</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>46</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="D57" s="33"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="H67"/>
       <c r="I67"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="D70" s="33"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>80</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
         <v>81</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>82</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>83</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
         <v>84</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
         <v>85</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
         <v>86</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
         <v>87</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>88</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
         <v>89</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="22" t="s">
         <v>100</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="22" t="s">
         <v>101</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="22" t="s">
         <v>102</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="22" t="s">
         <v>103</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="22" t="s">
         <v>104</v>
       </c>
@@ -3116,7 +3116,7 @@
       <c r="H106" s="17"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
         <v>105</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="22" t="s">
         <v>106</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="22" t="s">
         <v>107</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
         <v>108</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="22" t="s">
         <v>109</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="22" t="s">
         <v>110</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="31" t="s">
         <v>126</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="31" t="s">
         <v>127</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="31" t="s">
         <v>128</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="31" t="s">
         <v>129</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="31" t="s">
         <v>130</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="31" t="s">
         <v>131</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="31" t="s">
         <v>132</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="31" t="s">
         <v>133</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="31" t="s">
         <v>134</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="31" t="s">
         <v>135</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="31" t="s">
         <v>136</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="31" t="s">
         <v>137</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="30" t="s">
         <v>138</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="30" t="s">
         <v>139</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="30" t="s">
         <v>140</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="30" t="s">
         <v>141</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="30" t="s">
         <v>142</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="30" t="s">
         <v>143</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="30" t="s">
         <v>144</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="30" t="s">
         <v>145</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="30" t="s">
         <v>146</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="30" t="s">
         <v>147</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="30" t="s">
         <v>148</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="30" t="s">
         <v>149</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
         <v>152</v>
       </c>
@@ -3547,7 +3547,7 @@
       <c r="H154" s="17"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>159</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>162</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>163</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>164</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>165</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>167</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>168</v>
       </c>
@@ -3686,31 +3686,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E549543F-5A22-4ACD-8BC8-2DE808883B7A}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="23"/>
-    <col min="2" max="2" width="48.21875" style="23" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="13"/>
-    <col min="7" max="8" width="8.88671875" style="23"/>
-    <col min="9" max="9" width="9.109375"/>
-    <col min="10" max="10" width="8.88671875" style="23"/>
-    <col min="11" max="11" width="53.6640625" style="23" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="23"/>
+    <col min="1" max="1" width="8.85546875" style="23"/>
+    <col min="2" max="2" width="48.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="13"/>
+    <col min="7" max="8" width="8.85546875" style="23"/>
+    <col min="9" max="9" width="9.140625"/>
+    <col min="10" max="10" width="8.85546875" style="23"/>
+    <col min="11" max="11" width="53.7109375" style="23" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>209</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>337</v>
       </c>
@@ -3746,8 +3746,14 @@
       <c r="E2" s="26" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P2" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>338</v>
       </c>
@@ -3758,8 +3764,16 @@
         <v>338</v>
       </c>
       <c r="L3" s="28"/>
-    </row>
-    <row r="4" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P3"/>
+      <c r="Q3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="R3" s="15"/>
+      <c r="S3" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>339</v>
       </c>
@@ -3772,8 +3786,14 @@
       <c r="G4" s="23" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P4"/>
+      <c r="Q4" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="R4" s="15"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>340</v>
       </c>
@@ -3783,8 +3803,10 @@
       <c r="C5" s="24" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="24"/>
+      <c r="S5" s="25"/>
+    </row>
+    <row r="6" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>341</v>
       </c>
@@ -3794,8 +3816,16 @@
       <c r="C6" s="24" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P6"/>
+      <c r="Q6" t="s">
+        <v>244</v>
+      </c>
+      <c r="R6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S6" s="25"/>
+    </row>
+    <row r="7" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>342</v>
       </c>
@@ -3806,7 +3836,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>343</v>
       </c>
@@ -3817,7 +3847,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>344</v>
       </c>
@@ -3828,7 +3858,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>345</v>
       </c>
@@ -3839,7 +3869,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>346</v>
       </c>
@@ -3850,7 +3880,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>347</v>
       </c>
@@ -3861,7 +3891,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>348</v>
       </c>
@@ -3872,7 +3902,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>349</v>
       </c>
@@ -3883,7 +3913,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>350</v>
       </c>
@@ -3894,7 +3924,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>351</v>
       </c>
@@ -3905,7 +3935,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>352</v>
       </c>
@@ -3916,7 +3946,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>353</v>
       </c>
@@ -3927,71 +3957,13 @@
         <v>353</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H21" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="I21" s="32"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H22"/>
-      <c r="I22" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="L22" s="26"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H23"/>
-      <c r="I23" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="26"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H25"/>
-      <c r="I25" t="s">
-        <v>244</v>
-      </c>
-      <c r="J25" t="s">
-        <v>245</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I26" s="23"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="26"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="H25 A27:A28">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="Q6">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="P6">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4006,14 +3978,14 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="7" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>169</v>
       </c>
@@ -4021,7 +3993,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -4030,7 +4002,7 @@
       </c>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -4038,7 +4010,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
@@ -4046,7 +4018,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>59</v>
       </c>
@@ -4054,7 +4026,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>77</v>
       </c>
@@ -4062,7 +4034,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
@@ -4070,7 +4042,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -4078,7 +4050,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
@@ -4086,7 +4058,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>88</v>
       </c>
@@ -4094,7 +4066,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>99</v>
       </c>
@@ -4102,7 +4074,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>108</v>
       </c>
@@ -4110,7 +4082,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>114</v>
       </c>
@@ -4118,7 +4090,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>115</v>
       </c>
@@ -4127,7 +4099,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>152</v>
       </c>
@@ -4135,7 +4107,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>153</v>
       </c>
@@ -4143,7 +4115,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>154</v>
       </c>
@@ -4151,7 +4123,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>156</v>
       </c>
@@ -4159,7 +4131,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>157</v>
       </c>
@@ -4167,7 +4139,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>158</v>
       </c>
@@ -4175,7 +4147,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>160</v>
       </c>
@@ -4183,7 +4155,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>161</v>
       </c>
@@ -4191,7 +4163,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>167</v>
       </c>
@@ -4199,7 +4171,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>168</v>
       </c>
@@ -4218,67 +4190,67 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F18"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A10 A19:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4289,21 +4261,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631D602C-6727-4924-8375-43BF471931BB}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" customWidth="1"/>
-    <col min="5" max="5" width="52.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="52.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>502</v>
       </c>
@@ -4323,7 +4295,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>396</v>
       </c>
@@ -4343,7 +4315,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>397</v>
       </c>
@@ -4361,7 +4333,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>398</v>
       </c>
@@ -4375,7 +4347,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>399</v>
       </c>
@@ -4389,7 +4361,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>400</v>
       </c>
@@ -4403,7 +4375,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>401</v>
       </c>
@@ -4417,7 +4389,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>441</v>
       </c>
@@ -4431,7 +4403,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>444</v>
       </c>
@@ -4445,7 +4417,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -4457,7 +4429,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -4469,7 +4441,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="37"/>
       <c r="C12" s="37"/>
@@ -4481,7 +4453,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -4493,7 +4465,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="37"/>
       <c r="C14" s="37"/>
@@ -4505,7 +4477,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -4517,7 +4489,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -4529,7 +4501,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -4541,7 +4513,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -4553,7 +4525,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -4565,7 +4537,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
@@ -4577,7 +4549,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -4589,7 +4561,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
@@ -4601,7 +4573,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -4613,7 +4585,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -4625,7 +4597,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>

</xml_diff>

<commit_message>
Implemented marking of stemmed text and preserving the formatting, implemented verbose output of null counts, implemented reading from txt files, added console messages for succesful creation of jsonfiles and end of mapping
</commit_message>
<xml_diff>
--- a/keywords/keywords.xlsx
+++ b/keywords/keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_JRC\Mapping_2\Keywords\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\SDG\Policy-Mapping\keywords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EB7C7-91C0-4A33-9689-A106948B7AF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F01615-3BE2-4C2A-B3E7-D1DA3AFF051A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target_keys" sheetId="1" r:id="rId1"/>
@@ -2172,20 +2172,20 @@
       <selection pane="bottomRight" activeCell="B61" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="12" customWidth="1"/>
     <col min="5" max="5" width="18" style="17" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="12" customWidth="1"/>
     <col min="8" max="8" width="18" style="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>169</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>3</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>5</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>6</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>15</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>16</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>17</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>18</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>19</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>20</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>21</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>22</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>23</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>24</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>25</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>27</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>28</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>29</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>30</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>31</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>32</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>33</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>34</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>35</v>
       </c>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>36</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>37</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>38</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>39</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>40</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>41</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>42</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>43</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>44</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>45</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
         <v>46</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="D57" s="33"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="H67"/>
       <c r="I67"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="D70" s="33"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="19" t="s">
         <v>80</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="19" t="s">
         <v>81</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
         <v>82</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
         <v>83</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
         <v>84</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
         <v>85</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
         <v>86</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
         <v>87</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>88</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
         <v>89</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="22" t="s">
         <v>100</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="22" t="s">
         <v>101</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="22" t="s">
         <v>102</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="22" t="s">
         <v>103</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="22" t="s">
         <v>104</v>
       </c>
@@ -3116,7 +3116,7 @@
       <c r="H106" s="17"/>
       <c r="I106" s="13"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
         <v>105</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="22" t="s">
         <v>106</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="22" t="s">
         <v>107</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="22" t="s">
         <v>108</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="22" t="s">
         <v>109</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="22" t="s">
         <v>110</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="31" t="s">
         <v>126</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="31" t="s">
         <v>127</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="31" t="s">
         <v>128</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="31" t="s">
         <v>129</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="31" t="s">
         <v>130</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="31" t="s">
         <v>131</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="31" t="s">
         <v>132</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="31" t="s">
         <v>133</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="31" t="s">
         <v>134</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="31" t="s">
         <v>135</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="31" t="s">
         <v>136</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="31" t="s">
         <v>137</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="30" t="s">
         <v>138</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="30" t="s">
         <v>139</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="30" t="s">
         <v>140</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="30" t="s">
         <v>141</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="30" t="s">
         <v>142</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="30" t="s">
         <v>143</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="30" t="s">
         <v>144</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="30" t="s">
         <v>145</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="30" t="s">
         <v>146</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="30" t="s">
         <v>147</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="30" t="s">
         <v>148</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="30" t="s">
         <v>149</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
         <v>152</v>
       </c>
@@ -3547,7 +3547,7 @@
       <c r="H154" s="17"/>
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>159</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>162</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>163</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>164</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>165</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>167</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>168</v>
       </c>
@@ -3686,31 +3686,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E549543F-5A22-4ACD-8BC8-2DE808883B7A}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="23"/>
-    <col min="2" max="2" width="48.21875" style="23" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="25" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="13"/>
-    <col min="7" max="8" width="8.88671875" style="23"/>
-    <col min="9" max="9" width="9.109375"/>
-    <col min="10" max="10" width="8.88671875" style="23"/>
-    <col min="11" max="11" width="53.6640625" style="23" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="23"/>
+    <col min="1" max="1" width="8.85546875" style="23"/>
+    <col min="2" max="2" width="48.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="13"/>
+    <col min="7" max="8" width="8.85546875" style="23"/>
+    <col min="9" max="9" width="9.140625"/>
+    <col min="10" max="10" width="8.85546875" style="23"/>
+    <col min="11" max="11" width="53.7109375" style="23" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>209</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>337</v>
       </c>
@@ -3746,8 +3746,14 @@
       <c r="E2" s="26" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P2" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>338</v>
       </c>
@@ -3758,8 +3764,16 @@
         <v>338</v>
       </c>
       <c r="L3" s="28"/>
-    </row>
-    <row r="4" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P3"/>
+      <c r="Q3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="R3" s="15"/>
+      <c r="S3" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>339</v>
       </c>
@@ -3772,8 +3786,14 @@
       <c r="G4" s="23" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P4"/>
+      <c r="Q4" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="R4" s="15"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>340</v>
       </c>
@@ -3783,8 +3803,10 @@
       <c r="C5" s="24" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="24"/>
+      <c r="S5" s="25"/>
+    </row>
+    <row r="6" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
         <v>341</v>
       </c>
@@ -3794,8 +3816,16 @@
       <c r="C6" s="24" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P6"/>
+      <c r="Q6" t="s">
+        <v>244</v>
+      </c>
+      <c r="R6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S6" s="25"/>
+    </row>
+    <row r="7" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>342</v>
       </c>
@@ -3806,7 +3836,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
         <v>343</v>
       </c>
@@ -3817,7 +3847,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>344</v>
       </c>
@@ -3828,7 +3858,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>345</v>
       </c>
@@ -3839,7 +3869,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>346</v>
       </c>
@@ -3850,7 +3880,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
         <v>347</v>
       </c>
@@ -3861,7 +3891,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>348</v>
       </c>
@@ -3872,7 +3902,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>349</v>
       </c>
@@ -3883,7 +3913,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
         <v>350</v>
       </c>
@@ -3894,7 +3924,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>351</v>
       </c>
@@ -3905,7 +3935,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
         <v>352</v>
       </c>
@@ -3916,7 +3946,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>353</v>
       </c>
@@ -3927,71 +3957,13 @@
         <v>353</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H21" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="I21" s="32"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="26"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H22"/>
-      <c r="I22" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="L22" s="26"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H23"/>
-      <c r="I23" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="26"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="26"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H25"/>
-      <c r="I25" t="s">
-        <v>244</v>
-      </c>
-      <c r="J25" t="s">
-        <v>245</v>
-      </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="26"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I26" s="23"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="26"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="H25 A27:A28">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="Q6">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I25">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="P6">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4006,14 +3978,14 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="7" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>169</v>
       </c>
@@ -4021,7 +3993,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -4030,7 +4002,7 @@
       </c>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -4038,7 +4010,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
@@ -4046,7 +4018,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>59</v>
       </c>
@@ -4054,7 +4026,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>77</v>
       </c>
@@ -4062,7 +4034,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>78</v>
       </c>
@@ -4070,7 +4042,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -4078,7 +4050,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
@@ -4086,7 +4058,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>88</v>
       </c>
@@ -4094,7 +4066,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>99</v>
       </c>
@@ -4102,7 +4074,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>108</v>
       </c>
@@ -4110,7 +4082,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>114</v>
       </c>
@@ -4118,7 +4090,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>115</v>
       </c>
@@ -4127,7 +4099,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>152</v>
       </c>
@@ -4135,7 +4107,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>153</v>
       </c>
@@ -4143,7 +4115,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>154</v>
       </c>
@@ -4151,7 +4123,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>156</v>
       </c>
@@ -4159,7 +4131,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>157</v>
       </c>
@@ -4167,7 +4139,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>158</v>
       </c>
@@ -4175,7 +4147,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>160</v>
       </c>
@@ -4183,7 +4155,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>161</v>
       </c>
@@ -4191,7 +4163,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>167</v>
       </c>
@@ -4199,7 +4171,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>168</v>
       </c>
@@ -4218,67 +4190,67 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F18"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A10 A19:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4289,21 +4261,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631D602C-6727-4924-8375-43BF471931BB}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" customWidth="1"/>
-    <col min="5" max="5" width="52.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="52.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>502</v>
       </c>
@@ -4323,7 +4295,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>396</v>
       </c>
@@ -4343,7 +4315,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>397</v>
       </c>
@@ -4361,7 +4333,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>398</v>
       </c>
@@ -4375,7 +4347,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
         <v>399</v>
       </c>
@@ -4389,7 +4361,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>400</v>
       </c>
@@ -4403,7 +4375,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>401</v>
       </c>
@@ -4417,7 +4389,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
         <v>441</v>
       </c>
@@ -4431,7 +4403,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>444</v>
       </c>
@@ -4445,7 +4417,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -4457,7 +4429,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -4469,7 +4441,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="37"/>
       <c r="C12" s="37"/>
@@ -4481,7 +4453,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="37"/>
       <c r="C13" s="37"/>
@@ -4493,7 +4465,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="37"/>
       <c r="C14" s="37"/>
@@ -4505,7 +4477,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
@@ -4517,7 +4489,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
       <c r="B16" s="37"/>
       <c r="C16" s="37"/>
@@ -4529,7 +4501,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
@@ -4541,7 +4513,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
       <c r="B18" s="37"/>
       <c r="C18" s="37"/>
@@ -4553,7 +4525,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
       <c r="B19" s="37"/>
       <c r="C19" s="37"/>
@@ -4565,7 +4537,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
@@ -4577,7 +4549,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
@@ -4589,7 +4561,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="37"/>
       <c r="C22" s="37"/>
@@ -4601,7 +4573,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
@@ -4613,7 +4585,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -4625,7 +4597,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>

</xml_diff>